<commit_message>
feat(whatsapp-bot): optimización de velocidad y fiabilidad en envío de mensajesImplementa una estrategia optimizada para envío de mensajes en WhatsApp Web:- Reemplaza esperas fijas por detección dinámica de elementos- Corrige selección del campo de texto usando selectores específicos de chat- Implementa sistema de fallback para casos de error- Reduce tiempos entre operaciones secuenciales- Mejora detección de ventanas emergentes- Reduce tiempo de procesamiento por mensaje de >60s a ~15sEsta versión estable garantiza envíos confiables y significativamentemás rápidos, con mejor manejo de errores y capturas diagnósticas.
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Desktop\MensajesAutomaticos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Desktop\MensajesAutomaticos\messaging-automation-suite\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8074332-EE73-4D28-BAAB-FC96EFA46D26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1F8EDD-FE4C-4EA7-8496-23138F85446B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Nombre</t>
   </si>
@@ -36,35 +36,47 @@
     <t>Deuda</t>
   </si>
   <si>
-    <t>Cedula</t>
-  </si>
-  <si>
     <t>Telefono</t>
   </si>
   <si>
-    <t>Camilo</t>
-  </si>
-  <si>
-    <t>Catalina</t>
-  </si>
-  <si>
-    <t>Galindo</t>
-  </si>
-  <si>
-    <t>Suarez</t>
-  </si>
-  <si>
-    <t>Anggie</t>
-  </si>
-  <si>
-    <t>Espitia</t>
+    <t>CAMILO</t>
+  </si>
+  <si>
+    <t>GALINDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARLOS </t>
+  </si>
+  <si>
+    <t>RAMIREZ</t>
+  </si>
+  <si>
+    <t>CATALINA</t>
+  </si>
+  <si>
+    <t>SUAREZ</t>
+  </si>
+  <si>
+    <t>JAIME</t>
+  </si>
+  <si>
+    <t>SEBASTIAN</t>
+  </si>
+  <si>
+    <t>ANGGIE</t>
+  </si>
+  <si>
+    <t>ESPITIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,10 +91,23 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF404040"/>
-      <name val="Segoe UI"/>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="SansSerif"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="SansSerif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,23 +127,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 31" xfId="1" xr:uid="{6430EED1-B3DB-4796-B453-8C7AD62684E5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -396,22 +441,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,77 +468,198 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="7">
+        <v>120000</v>
+      </c>
+      <c r="D2" s="6">
+        <v>3204886934</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7">
+        <v>130000</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3238109564</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
-        <v>300000</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1052416519</v>
-      </c>
-      <c r="E2" s="2">
-        <v>573204886934</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C4" s="7">
+        <v>140000</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3204886934</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15">
+      <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
+      <c r="B5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7">
         <v>150000</v>
       </c>
-      <c r="D3" s="2">
-        <v>46450309</v>
-      </c>
-      <c r="E3" s="2">
-        <v>573144708305</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>299999</v>
-      </c>
-      <c r="D4">
-        <v>46450309</v>
-      </c>
-      <c r="E4">
-        <v>573132832558</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D5" s="6">
+        <v>3144708305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15">
+      <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>324567</v>
-      </c>
-      <c r="D5">
-        <v>1052410306</v>
-      </c>
-      <c r="E5">
-        <v>573238109564</v>
-      </c>
+      <c r="B6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7">
+        <v>160000</v>
+      </c>
+      <c r="D6" s="6">
+        <v>3103332475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7">
+        <v>170000</v>
+      </c>
+      <c r="D7" s="6">
+        <v>3153078903</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="15">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="15">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="15">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="15">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="15">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="15">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="15">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="15">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="15">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="15">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="15">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="15">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="15">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="15">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="15">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="15">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="15">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: preservar saltos de línea en mensajes de WhatsApp usando ActionChains
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Desktop\MensajesAutomaticos\messaging-automation-suite\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1F8EDD-FE4C-4EA7-8496-23138F85446B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955B58F0-DF31-4F79-9F2B-5716572B29D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -494,7 +494,7 @@
         <v>130000</v>
       </c>
       <c r="D3" s="6">
-        <v>3238109564</v>
+        <v>3204886934</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15">
@@ -522,7 +522,7 @@
         <v>150000</v>
       </c>
       <c r="D5" s="6">
-        <v>3144708305</v>
+        <v>3204886934</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15">
@@ -536,7 +536,7 @@
         <v>160000</v>
       </c>
       <c r="D6" s="6">
-        <v>3103332475</v>
+        <v>3204886934</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15">
@@ -550,7 +550,7 @@
         <v>170000</v>
       </c>
       <c r="D7" s="6">
-        <v>3153078903</v>
+        <v>3204886934</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15">

</xml_diff>